<commit_message>
Day3 end and Day4 start
Designing end and Testing start
</commit_message>
<xml_diff>
--- a/Production/Dark World Development File 3.0.xlsx
+++ b/Production/Dark World Development File 3.0.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113">
   <si>
     <t>Control</t>
   </si>
@@ -329,26 +329,10 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Level Design and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">;
-Optimize the exist level;
+      <t xml:space="preserve">Combin Scene and Triggers;
+Niko:1st Floor;
+Hugo:2nd Floor;
+Hank:3rd Floor;
 </t>
     </r>
     <r>
@@ -358,7 +342,7 @@
         <rFont val="Verdana"/>
         <charset val="134"/>
       </rPr>
-      <t>Musician Parts</t>
+      <t>Musician Parts(kiki)</t>
     </r>
     <r>
       <rPr>
@@ -378,6 +362,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <charset val="134"/>
+      </rPr>
       <t>Core Mechanism Program</t>
     </r>
     <r>
@@ -430,13 +420,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Program</t>
+      <t>Program(John)</t>
     </r>
     <r>
       <rPr>
@@ -456,7 +440,7 @@
         <rFont val="Verdana"/>
         <charset val="134"/>
       </rPr>
-      <t>UI</t>
+      <t>UI(Leon)</t>
     </r>
     <r>
       <rPr>
@@ -466,7 +450,7 @@
         <charset val="134"/>
       </rPr>
       <t>:
-Ingame UI(Partical System)</t>
+Ingame UI</t>
     </r>
   </si>
   <si>
@@ -477,6 +461,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Verdana"/>
+        <charset val="134"/>
+      </rPr>
       <t>Ingame</t>
     </r>
     <r>
@@ -503,9 +493,13 @@
         <charset val="134"/>
       </rPr>
       <t>:
-Animation(KiKi, Neo);
 Element,Character Model(Raibeart)</t>
     </r>
+  </si>
+  <si>
+    <t>Start Animation(Neo)
+End Animation(kiki)
+Optimize the exist Level(Raibeart)</t>
   </si>
   <si>
     <t>Demand of Designer</t>
@@ -519,10 +513,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -599,6 +593,105 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -622,105 +715,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -781,6 +775,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -805,85 +925,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,18 +937,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -925,43 +955,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,30 +1069,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1110,6 +1080,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1164,6 +1143,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1178,10 +1172,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1190,137 +1184,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,21 +1329,18 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1392,21 +1383,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1433,12 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1458,9 +1428,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1836,146 +1803,146 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16.75" style="47" customWidth="1"/>
-    <col min="2" max="2" width="24.3333333333333" style="19" customWidth="1"/>
-    <col min="3" max="3" width="24.3333333333333" style="20" customWidth="1"/>
-    <col min="4" max="4" width="96.6666666666667" style="48" customWidth="1"/>
-    <col min="5" max="16383" width="8.88333333333333" style="31"/>
-    <col min="16384" max="16384" width="9" style="31"/>
+    <col min="1" max="1" width="16.75" style="39" customWidth="1"/>
+    <col min="2" max="2" width="24.3333333333333" style="18" customWidth="1"/>
+    <col min="3" max="3" width="24.3333333333333" style="19" customWidth="1"/>
+    <col min="4" max="4" width="96.6666666666667" style="32" customWidth="1"/>
+    <col min="5" max="16383" width="8.88333333333333" style="25"/>
+    <col min="16384" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" ht="20.25" spans="1:4">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="20.25" spans="1:4">
-      <c r="A5" s="14"/>
-      <c r="B5" s="45" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="45" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" ht="20.25" spans="1:4">
-      <c r="A6" s="14"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" ht="20.25" spans="1:4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="45" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" ht="20.25" spans="1:4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" ht="20.25" spans="1:4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" ht="20.25" spans="1:4">
-      <c r="A10" s="14"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" ht="20.25" spans="1:4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" ht="20.25" spans="1:4">
-      <c r="A12" s="14"/>
-      <c r="B12" s="45" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2001,370 +1968,370 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="8.88333333333333" style="32"/>
-    <col min="3" max="3" width="20.25" style="32" customWidth="1"/>
-    <col min="4" max="4" width="53.6666666666667" style="33" customWidth="1"/>
-    <col min="5" max="5" width="34.3333333333333" style="32" customWidth="1"/>
+    <col min="1" max="1" width="18.625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="8.88333333333333" style="26"/>
+    <col min="3" max="3" width="20.25" style="26" customWidth="1"/>
+    <col min="4" max="4" width="53.6666666666667" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.3333333333333" style="26" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="23.3333333333333" style="32" customWidth="1"/>
-    <col min="8" max="8" width="16.3333333333333" style="32" customWidth="1"/>
-    <col min="9" max="9" width="23.3333333333333" style="32" customWidth="1"/>
-    <col min="10" max="16381" width="8.88333333333333" style="32"/>
-    <col min="16382" max="16384" width="9" style="32"/>
+    <col min="7" max="7" width="23.3333333333333" style="26" customWidth="1"/>
+    <col min="8" max="8" width="16.3333333333333" style="26" customWidth="1"/>
+    <col min="9" max="9" width="23.3333333333333" style="26" customWidth="1"/>
+    <col min="10" max="16381" width="8.88333333333333" style="26"/>
+    <col min="16382" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="1" ht="19.8" customHeight="1" spans="1:10">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="24" customFormat="1" ht="19.8" customHeight="1" spans="1:10">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="43"/>
-    </row>
-    <row r="2" s="14" customFormat="1" ht="21" customHeight="1" spans="6:10">
-      <c r="F2" s="34"/>
-      <c r="G2" s="14" t="s">
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" s="13" customFormat="1" ht="21" customHeight="1" spans="6:10">
+      <c r="F2" s="28"/>
+      <c r="G2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="44"/>
-    </row>
-    <row r="3" s="19" customFormat="1" ht="31.5" customHeight="1" spans="1:10">
-      <c r="A3" s="19" t="s">
+      <c r="J2" s="36"/>
+    </row>
+    <row r="3" s="18" customFormat="1" ht="31.5" customHeight="1" spans="1:10">
+      <c r="A3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="J3" s="45"/>
-    </row>
-    <row r="4" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B4" s="19">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="45"/>
-    </row>
-    <row r="5" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B5" s="19">
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B5" s="18">
         <v>3</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="45"/>
-    </row>
-    <row r="6" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B6" s="19">
+      <c r="J5" s="37"/>
+    </row>
+    <row r="6" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B6" s="18">
         <v>4</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="45"/>
-    </row>
-    <row r="7" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B7" s="19">
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B7" s="18">
         <v>5</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B8" s="19">
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B8" s="18">
         <v>6</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="45"/>
-    </row>
-    <row r="9" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B9" s="19">
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B9" s="18">
         <v>7</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="45"/>
-    </row>
-    <row r="10" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B10" s="19">
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B10" s="18">
         <v>8</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="J10" s="45"/>
-    </row>
-    <row r="11" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B11" s="19">
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B11" s="18">
         <v>9</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="45"/>
-    </row>
-    <row r="12" s="19" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
-      <c r="B12" s="19">
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" s="18" customFormat="1" ht="31.5" customHeight="1" spans="2:10">
+      <c r="B12" s="18">
         <v>10</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="J12" s="45"/>
-    </row>
-    <row r="13" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
-      <c r="A13" s="19" t="s">
+      <c r="F12" s="31"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
+      <c r="A13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>11</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-    </row>
-    <row r="15" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
-      <c r="A15" s="38" t="s">
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:9">
+      <c r="A15" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-    </row>
-    <row r="16" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18">
         <v>12</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39">
+    <row r="17" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18">
         <v>13</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" s="31" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39">
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" s="25" customFormat="1" ht="31.5" customHeight="1" spans="1:6">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18">
         <v>14</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" s="31" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
-      <c r="D19" s="41"/>
-    </row>
-    <row r="20" s="31" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
-      <c r="D20" s="41"/>
-    </row>
-    <row r="21" s="31" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
-      <c r="D21" s="41"/>
-    </row>
-    <row r="22" s="31" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
-      <c r="D22" s="41"/>
-    </row>
-    <row r="23" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D23" s="41"/>
-      <c r="F23" s="42"/>
-    </row>
-    <row r="24" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D24" s="41"/>
-      <c r="F24" s="42"/>
-    </row>
-    <row r="25" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D25" s="41"/>
-      <c r="F25" s="42"/>
-    </row>
-    <row r="26" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D26" s="41"/>
-      <c r="F26" s="42"/>
-    </row>
-    <row r="27" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D27" s="41"/>
-      <c r="F27" s="42"/>
-    </row>
-    <row r="28" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D28" s="41"/>
-      <c r="F28" s="42"/>
-    </row>
-    <row r="29" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D29" s="41"/>
-      <c r="F29" s="42"/>
-    </row>
-    <row r="30" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D30" s="41"/>
-      <c r="F30" s="42"/>
-    </row>
-    <row r="31" s="31" customFormat="1" ht="20.25" spans="4:6">
-      <c r="D31" s="41"/>
-      <c r="F31" s="42"/>
+    <row r="19" s="25" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
+      <c r="D19" s="33"/>
+    </row>
+    <row r="20" s="25" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
+      <c r="D20" s="33"/>
+    </row>
+    <row r="21" s="25" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
+      <c r="D21" s="33"/>
+    </row>
+    <row r="22" s="25" customFormat="1" ht="31.5" customHeight="1" spans="4:4">
+      <c r="D22" s="33"/>
+    </row>
+    <row r="23" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D23" s="33"/>
+      <c r="F23" s="34"/>
+    </row>
+    <row r="24" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D24" s="33"/>
+      <c r="F24" s="34"/>
+    </row>
+    <row r="25" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D25" s="33"/>
+      <c r="F25" s="34"/>
+    </row>
+    <row r="26" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D26" s="33"/>
+      <c r="F26" s="34"/>
+    </row>
+    <row r="27" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D27" s="33"/>
+      <c r="F27" s="34"/>
+    </row>
+    <row r="28" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D28" s="33"/>
+      <c r="F28" s="34"/>
+    </row>
+    <row r="29" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D29" s="33"/>
+      <c r="F29" s="34"/>
+    </row>
+    <row r="30" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D30" s="33"/>
+      <c r="F30" s="34"/>
+    </row>
+    <row r="31" s="25" customFormat="1" ht="20.25" spans="4:6">
+      <c r="D31" s="33"/>
+      <c r="F31" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -2413,191 +2380,191 @@
   </cols>
   <sheetData>
     <row r="1" ht="59" customHeight="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" ht="21" spans="1:11">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" ht="20.25" spans="1:11">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" ht="45" customHeight="1" spans="1:11">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" ht="40.5" spans="1:11">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" ht="54" customHeight="1" spans="1:11">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" ht="53" customHeight="1" spans="1:11">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>4</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" ht="53" customHeight="1" spans="1:11">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <v>5</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" ht="51" customHeight="1" spans="1:11">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>6</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" ht="20.25" spans="5:6">
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" ht="20.25" spans="5:6">
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" ht="20.25" spans="5:6">
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" ht="20.25" spans="5:6">
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" ht="20.25" spans="5:6">
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2624,7 +2591,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -2676,21 +2643,21 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="8" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" ht="90" customHeight="1" spans="1:14">
       <c r="A3" s="4"/>
@@ -2698,41 +2665,41 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" customHeight="1" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" ht="85" customHeight="1" spans="1:14">
       <c r="A5" s="4"/>
@@ -2740,15 +2707,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" customHeight="1" spans="1:14">
       <c r="A6" s="4" t="s">
@@ -2760,21 +2727,21 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" ht="82" customHeight="1" spans="1:14">
       <c r="A7" s="4"/>
@@ -2782,19 +2749,19 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="9" customHeight="1" spans="2:2">
-      <c r="B9" s="11" t="s">
-        <v>111</v>
+      <c r="B9" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>